<commit_message>
Added Visual Studio to Tool Comparison
</commit_message>
<xml_diff>
--- a/Tools Comparison.xlsx
+++ b/Tools Comparison.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sheld.DESKTOP-JK1JFDM\Desktop\Baylor Sophomore\Intro to Computer System\Group Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sheld.DESKTOP-JK1JFDM\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19C6F140-36EB-4B21-AAC9-1F6BF327A8DE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB5E33FC-C165-46EB-A064-11CA519E28B7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{682F612F-D51C-4B09-AB0D-EE41E4AFC94F}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
   <si>
     <t>Tool Name</t>
   </si>
@@ -106,6 +106,24 @@
   </si>
   <si>
     <t>This program is pretty easy to use.  After playing around with the functions and seeing how it works, there is nothing difficult about it.</t>
+  </si>
+  <si>
+    <t>Visual Studio 2017</t>
+  </si>
+  <si>
+    <t>https://visualstudio.microsoft.com/downloads/</t>
+  </si>
+  <si>
+    <t>Debugger/IDE</t>
+  </si>
+  <si>
+    <t>Using the debugger with an executable can take a bit of time to get used to, but once you understand the basics it becomes easier.</t>
+  </si>
+  <si>
+    <t>This program allows the user to step through (trace) each line of the given  assembly code of the executable.  This can be very helpful to see how inputting different values changes the flow of the program.</t>
+  </si>
+  <si>
+    <t>Knowing how to upload an executable so that you can trace through it is not obvious and takes some time to find.</t>
   </si>
 </sst>
 </file>
@@ -173,7 +191,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -187,6 +205,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -505,15 +526,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C1CB59C-9B23-458A-B1E6-56E0879B651D}">
   <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="17.44140625" customWidth="1"/>
     <col min="2" max="2" width="25.88671875" customWidth="1"/>
-    <col min="3" max="3" width="24" customWidth="1"/>
+    <col min="3" max="3" width="40.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="25.109375" customWidth="1"/>
     <col min="5" max="5" width="30.77734375" customWidth="1"/>
     <col min="6" max="6" width="28.6640625" customWidth="1"/>
@@ -606,13 +627,25 @@
       </c>
       <c r="G4" s="5"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
+    <row r="5" spans="1:7" ht="111.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>29</v>
+      </c>
       <c r="G5" s="3"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -710,6 +743,7 @@
     <hyperlink ref="C4" r:id="rId1" xr:uid="{148BC509-4EF8-43DF-BF9A-3DA9FBE7253B}"/>
     <hyperlink ref="C2" r:id="rId2" xr:uid="{A47212DD-B072-4BF6-8C15-428C507D5B3C}"/>
     <hyperlink ref="C3" r:id="rId3" xr:uid="{B01188F3-3410-4F4A-8A59-DF7CABB96406}"/>
+    <hyperlink ref="C5" r:id="rId4" xr:uid="{1B423E48-03D7-4811-B789-0B7AD8B5458F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>